<commit_message>
pushing to github to transfer
</commit_message>
<xml_diff>
--- a/scraped.xlsx
+++ b/scraped.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="9180" yWindow="1180" windowWidth="19620" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,51 +27,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>http://www.1ne.org.uk/</t>
-  </si>
-  <si>
-    <t>http://facesinfocus.org.uk/</t>
-  </si>
-  <si>
-    <t>http://footstepsforfamilies.org/</t>
-  </si>
-  <si>
-    <t>http://healthyyoungmindspennine.nhs.uk/</t>
-  </si>
-  <si>
-    <t>http://interchangesheffield.org.uk/</t>
-  </si>
-  <si>
-    <t>http://kidstimefoundation.org/</t>
-  </si>
-  <si>
-    <t>http://otrtwickenham.com/</t>
-  </si>
-  <si>
-    <t>http://sayinggoodbye.org.uk/</t>
-  </si>
-  <si>
-    <t>http://sussexcommunity.org.uk/</t>
-  </si>
-  <si>
-    <t>http://thewishcentre.org.uk/</t>
-  </si>
-  <si>
-    <t>http://www.door-ways.co.uk/</t>
-  </si>
-  <si>
-    <t>http://www.cpchalifax.org.uk/</t>
-  </si>
-  <si>
-    <t>http://www.clivey.co.uk/</t>
-  </si>
-  <si>
-    <t>http://www.carefreekids.org/</t>
-  </si>
-  <si>
-    <t>http://welldoing.org/</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>http://www.youthtalk.org.uk/</t>
+  </si>
+  <si>
+    <t>http://www.womensaidnel.org/</t>
+  </si>
+  <si>
+    <t>http://www.swingsandsmiles.co.uk/</t>
+  </si>
+  <si>
+    <t>http://www.southendcarers.co.uk/</t>
+  </si>
+  <si>
+    <t>http://www.psspeople.com/</t>
+  </si>
+  <si>
+    <t>http://www.no-secrets.org.uk/</t>
+  </si>
+  <si>
+    <t>http://www.mindincroydon.org.uk/</t>
+  </si>
+  <si>
+    <t>http://www.middlesbroughandstocktonmind.org.uk/</t>
+  </si>
+  <si>
+    <t>https://www.ymcadlg.org/</t>
+  </si>
+  <si>
+    <t>https://www.place2be.org.uk/</t>
+  </si>
+  <si>
+    <t>https://www.kidscape.org.uk/</t>
+  </si>
+  <si>
+    <t>https://www.disc-vol.org.uk/</t>
   </si>
 </sst>
 </file>
@@ -386,87 +377,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A2:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A15"/>
+      <selection activeCell="A9" sqref="A9:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>